<commit_message>
changed the data for metric 6 in Lang into a new one
</commit_message>
<xml_diff>
--- a/data/Apache commons Lang 79.8K/BMI/Metric 6-Lang.xlsx
+++ b/data/Apache commons Lang 79.8K/BMI/Metric 6-Lang.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21425"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{538357B4-4AA7-4A90-926D-A6B04B6F0DD0}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6C4878FE-4F01-4632-A5F4-824D2D6ECEA5}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="5376" yWindow="1296" windowWidth="12576" windowHeight="8976" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="10668" yWindow="1548" windowWidth="12576" windowHeight="8976" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -52,31 +52,32 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>project = LANG AND issuetype = Bug AND  affectedVersion in (1.0,2.0) AND status = Closed  AND createdDate &gt; "2000/11/24" ORDER BY created DESC</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>Version Coverage</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>1.0~2.0（1.0，1.0.1）</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>2.0~3.0（2.0，2.1，2.2，2.3，2.4，2.5，2.6）</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>3.0~3.8.1（3.0，3.1，3.2，3.2.1，3.3，3.3.1，3.3.2，3.4，3.5，3.6，3.8，3.8.1）</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>Date</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>https://issues.apache.org/jira/secure/ConfigureReport.jspa?projectOrFilterId=project-12310481&amp;dateField=created&amp;periodName=monthly&amp;daysprevious=7200&amp;cumulative=true&amp;selectedProjectId=12310481&amp;reportKey=com.atlassian.jira.jira-core-reports-plugin%3Atimesince-report&amp;atl_token=A5KQ-2QAV-T4JA-FDED%7C2e411ca6e9b41de8c75e4366f0363a384cbb1fdf%7Clout&amp;Next=Next</t>
+    <t>3.0~3.6</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>3.6~3.7</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>3.7~3.8</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>project = LANG AND issuetype = Bug AND  affectedVersion in (3.0,3.6) AND status = Closed  AND createdDate &gt; "2011/01/01" ORDER BY created DESC</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>https://issues.apache.org/jira/secure/ConfigureReport.jspa?projectOrFilterId=project-12310481&amp;dateField=created&amp;periodName=monthly&amp;daysprevious=7200&amp;cumulative=true&amp;selectedProjectId=12310481&amp;reportKey=com.atlassian.jira.jira-core-reports-plugin%3Atimesince-report&amp;atl_token=A5KQ-2QAV-T4JA-FDED%7C06b3f857d3c464eb55cc90414bee10b3a9f28b29%7Clout&amp;Next=Next</t>
+    <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
 </file>
@@ -131,9 +132,9 @@
   <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="17" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="17" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="常规" xfId="0" builtinId="0"/>
@@ -418,7 +419,7 @@
   <dimension ref="A1:M17"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D15" sqref="D15"/>
+      <selection activeCell="D17" sqref="D17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
@@ -428,7 +429,7 @@
   <sheetData>
     <row r="1" spans="1:13">
       <c r="A1" t="s">
-        <v>11</v>
+        <v>7</v>
       </c>
       <c r="B1" t="s">
         <v>5</v>
@@ -449,82 +450,82 @@
         <v>2</v>
       </c>
       <c r="H1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="2" spans="1:13">
-      <c r="A2" s="3">
-        <v>37622</v>
+      <c r="A2" s="2">
+        <v>40725</v>
       </c>
       <c r="B2">
-        <v>10</v>
+        <v>24</v>
       </c>
       <c r="C2">
-        <v>10</v>
+        <v>3</v>
       </c>
       <c r="D2">
         <f>(C2/B2)</f>
-        <v>1</v>
+        <v>0.125</v>
       </c>
       <c r="E2">
         <f>MAX(D2:D4)</f>
-        <v>1</v>
+        <v>0.2</v>
       </c>
       <c r="F2">
         <f>MIN(D2:D4)</f>
-        <v>0.2857142857142857</v>
+        <v>0</v>
       </c>
       <c r="G2">
         <f>AVERAGE(D2:D4)</f>
-        <v>0.5619047619047618</v>
+        <v>0.10833333333333334</v>
       </c>
       <c r="H2" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="3" spans="1:13">
-      <c r="A3" s="3">
-        <v>37653</v>
+      <c r="A3" s="2">
+        <v>40756</v>
       </c>
       <c r="B3">
-        <v>7</v>
+        <v>15</v>
       </c>
       <c r="C3">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="D3">
         <f t="shared" ref="D3:D10" si="0">(C3/B3)</f>
-        <v>0.2857142857142857</v>
+        <v>0.2</v>
       </c>
     </row>
     <row r="4" spans="1:13">
-      <c r="A4" s="3">
-        <v>37681</v>
+      <c r="A4" s="2">
+        <v>40787</v>
       </c>
       <c r="B4">
-        <v>5</v>
+        <v>8</v>
       </c>
       <c r="C4">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="D4">
         <f t="shared" si="0"/>
-        <v>0.4</v>
+        <v>0</v>
       </c>
     </row>
     <row r="5" spans="1:13">
-      <c r="A5" s="3">
-        <v>37865</v>
+      <c r="A5" s="2">
+        <v>42917</v>
       </c>
       <c r="B5">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="C5">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="D5">
         <f t="shared" si="0"/>
-        <v>0.8</v>
+        <v>0</v>
       </c>
       <c r="E5">
         <f>MAX(D5:D7)</f>
@@ -532,139 +533,139 @@
       </c>
       <c r="F5">
         <f>MIN(D5:D7)</f>
-        <v>0.25</v>
+        <v>0</v>
       </c>
       <c r="G5">
         <f>AVERAGE(D5:D7)</f>
-        <v>0.44523809523809527</v>
+        <v>0.43333333333333335</v>
       </c>
       <c r="H5" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="6" spans="1:13">
-      <c r="A6" s="3">
-        <v>37895</v>
+      <c r="A6" s="2">
+        <v>42948</v>
       </c>
       <c r="B6">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="C6">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="D6">
         <f t="shared" si="0"/>
-        <v>0.2857142857142857</v>
+        <v>0.8</v>
       </c>
     </row>
     <row r="7" spans="1:13">
-      <c r="A7" s="3">
-        <v>37926</v>
+      <c r="A7" s="2">
+        <v>42979</v>
       </c>
       <c r="B7">
         <v>4</v>
       </c>
       <c r="C7">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D7">
         <f t="shared" si="0"/>
-        <v>0.25</v>
+        <v>0.5</v>
       </c>
     </row>
     <row r="8" spans="1:13">
-      <c r="A8" s="3">
-        <v>40725</v>
+      <c r="A8" s="2">
+        <v>43101</v>
       </c>
       <c r="B8">
-        <v>24</v>
+        <v>5</v>
       </c>
       <c r="C8">
         <v>2</v>
       </c>
       <c r="D8">
         <f t="shared" si="0"/>
-        <v>8.3333333333333329E-2</v>
+        <v>0.4</v>
       </c>
       <c r="E8">
         <f>MAX(D8:D10)</f>
-        <v>8.3333333333333329E-2</v>
+        <v>0.4</v>
       </c>
       <c r="F8">
         <f>MIN(D8:D10)</f>
-        <v>0</v>
+        <v>0.2857142857142857</v>
       </c>
       <c r="G8">
         <f>AVERAGE(D8:D10)</f>
-        <v>4.9999999999999996E-2</v>
+        <v>0.33968253968253964</v>
       </c>
       <c r="H8" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="9" spans="1:13">
-      <c r="A9" s="3">
-        <v>40756</v>
+      <c r="A9" s="2">
+        <v>43132</v>
       </c>
       <c r="B9">
-        <v>15</v>
+        <v>3</v>
       </c>
       <c r="C9">
         <v>1</v>
       </c>
       <c r="D9">
         <f t="shared" si="0"/>
-        <v>6.6666666666666666E-2</v>
+        <v>0.33333333333333331</v>
       </c>
     </row>
     <row r="10" spans="1:13">
-      <c r="A10" s="3">
-        <v>40787</v>
+      <c r="A10" s="2">
+        <v>43160</v>
       </c>
       <c r="B10">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C10">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="D10">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>0.2857142857142857</v>
       </c>
     </row>
     <row r="12" spans="1:13">
-      <c r="A12" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="B12" s="2"/>
-      <c r="C12" s="2"/>
-      <c r="D12" s="2"/>
-      <c r="E12" s="2"/>
-      <c r="F12" s="2"/>
-      <c r="G12" s="2"/>
-      <c r="H12" s="2"/>
-      <c r="I12" s="2"/>
-      <c r="J12" s="2"/>
-      <c r="K12" s="2"/>
-      <c r="L12" s="2"/>
-      <c r="M12" s="2"/>
+      <c r="A12" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="B12" s="3"/>
+      <c r="C12" s="3"/>
+      <c r="D12" s="3"/>
+      <c r="E12" s="3"/>
+      <c r="F12" s="3"/>
+      <c r="G12" s="3"/>
+      <c r="H12" s="3"/>
+      <c r="I12" s="3"/>
+      <c r="J12" s="3"/>
+      <c r="K12" s="3"/>
+      <c r="L12" s="3"/>
+      <c r="M12" s="3"/>
     </row>
     <row r="13" spans="1:13">
       <c r="A13" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="B13" s="4"/>
-      <c r="C13" s="4"/>
-      <c r="D13" s="4"/>
-      <c r="E13" s="4"/>
-      <c r="F13" s="4"/>
-      <c r="G13" s="4"/>
-      <c r="H13" s="4"/>
-      <c r="I13" s="4"/>
-      <c r="J13" s="4"/>
-      <c r="K13" s="4"/>
-      <c r="L13" s="4"/>
-      <c r="M13" s="4"/>
+      <c r="B13" s="3"/>
+      <c r="C13" s="3"/>
+      <c r="D13" s="3"/>
+      <c r="E13" s="3"/>
+      <c r="F13" s="3"/>
+      <c r="G13" s="3"/>
+      <c r="H13" s="3"/>
+      <c r="I13" s="3"/>
+      <c r="J13" s="3"/>
+      <c r="K13" s="3"/>
+      <c r="L13" s="3"/>
+      <c r="M13" s="3"/>
     </row>
     <row r="16" spans="1:13">
       <c r="B16" s="1"/>
@@ -678,7 +679,10 @@
     <mergeCell ref="A13:M13"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
+  <hyperlinks>
+    <hyperlink ref="A13" r:id="rId1" display="https://issues.apache.org/jira/secure/ConfigureReport.jspa?projectOrFilterId=project-12310481&amp;dateField=created&amp;periodName=monthly&amp;daysprevious=7200&amp;cumulative=true&amp;selectedProjectId=12310481&amp;reportKey=com.atlassian.jira.jira-core-reports-plugin%3Atimesince-report&amp;atl_token=A5KQ-2QAV-T4JA-FDED%7C06b3f857d3c464eb55cc90414bee10b3a9f28b29%7Clout&amp;Next=Next" xr:uid="{876690BB-CE38-4615-951F-E06D78BBE946}"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId1"/>
+  <pageSetup orientation="portrait" r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>